<commit_message>
fixing scene type based filter
</commit_message>
<xml_diff>
--- a/Projects/GSKAU_SAND/Data/Secondary_Display_KPI_External_Targets.xlsx
+++ b/Projects/GSKAU_SAND/Data/Secondary_Display_KPI_External_Targets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t xml:space="preserve">Store Number</t>
   </si>
@@ -64,97 +64,70 @@
     <t xml:space="preserve">IND Grocery</t>
   </si>
   <si>
+    <t xml:space="preserve">Oberon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Australia</t>
   </si>
   <si>
+    <t xml:space="preserve">Mawhoods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floor Bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673834355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673836397</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673808172, 9300673800000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pharmacy</t>
+  </si>
+  <si>
     <t xml:space="preserve">T</t>
   </si>
   <si>
-    <t xml:space="preserve">Counter Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9310320000781</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9314057001400, 9314057006542</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9314057006535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pharmacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TORRENSVILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Floor Bin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9310130175938</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300633900595, 9334820000058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foodworks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALBURY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9310130037779</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grocery</t>
+    <t xml:space="preserve">Other0019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673854407, 9300673916792</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673923936, 9300673822109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castlecrag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romeos</t>
   </si>
   <si>
     <t xml:space="preserve">Gondola End</t>
   </si>
   <si>
-    <t xml:space="preserve">9310042275382</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673840479</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0019000001hGahUAAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673171863</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673879394, 9300673879561</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673851000, 9300673851011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673827203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673868343, 9300673834355, 9300673836397</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673827203, 9300673854742</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673840646</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673840813, 9300673854407</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673840646, 9300673854742, Other0007</t>
+    <t xml:space="preserve">9300673840134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9403099004590, Irrelevant0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673923936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673838773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9403099004590, 9300673840134</t>
   </si>
 </sst>
 </file>
@@ -276,7 +249,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -325,7 +298,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -339,10 +312,6 @@
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -423,31 +392,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:9"/>
+  <dimension ref="1:5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="30.4285714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="35.8469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="4" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="5" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="4" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="5" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="9" customFormat="true" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -494,25 +464,30 @@
       <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="D2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="12"/>
+        <v>15</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="F2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L2" s="15" t="n">
         <v>43648</v>
@@ -521,33 +496,31 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
       <c r="B3" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C3" s="14"/>
       <c r="D3" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="14" t="n">
-        <v>9300633682880</v>
+      <c r="H3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L3" s="15" t="n">
         <v>43648</v>
@@ -556,35 +529,35 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10"/>
-      <c r="B4" s="14" t="s">
-        <v>20</v>
+      <c r="B4" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="14" t="n">
-        <v>9300633682880</v>
+        <v>29</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="L4" s="15" t="n">
         <v>43648</v>
@@ -593,158 +566,32 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>27</v>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="14" t="n">
-        <v>9310130820005</v>
-      </c>
-      <c r="K5" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="L5" s="15" t="n">
         <v>43648</v>
       </c>
       <c r="M5" s="15" t="n">
-        <v>43682</v>
-      </c>
-    </row>
-    <row r="6" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
-      <c r="B6" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="14" t="n">
-        <v>9310130820005</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="15" t="n">
-        <v>43648</v>
-      </c>
-      <c r="M6" s="15" t="n">
-        <v>43682</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="15" t="n">
-        <v>43648</v>
-      </c>
-      <c r="M7" s="15" t="n">
-        <v>43682</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="15" t="n">
-        <v>43648</v>
-      </c>
-      <c r="M8" s="15" t="n">
-        <v>43682</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L9" s="15" t="n">
-        <v>43648</v>
-      </c>
-      <c r="M9" s="15" t="n">
         <v>43682</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding detailed sku kpi
</commit_message>
<xml_diff>
--- a/Projects/GSKAU_SAND/Data/Secondary_Display_KPI_External_Targets.xlsx
+++ b/Projects/GSKAU_SAND/Data/Secondary_Display_KPI_External_Targets.xlsx
@@ -395,26 +395,17 @@
   <dimension ref="1:5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="4" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="5" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="3" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="2" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="4" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="5" width="14.7244897959184"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,7 +450,7 @@
       </c>
       <c r="AMJ1" s="5"/>
     </row>
-    <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
         <v>13</v>
@@ -496,7 +487,7 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
       <c r="B3" s="14" t="s">
         <v>22</v>
@@ -529,7 +520,7 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>13</v>
@@ -566,7 +557,7 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
added kpi for detailed; fixed summary kpi
</commit_message>
<xml_diff>
--- a/Projects/GSKAU_SAND/Data/Secondary_Display_KPI_External_Targets.xlsx
+++ b/Projects/GSKAU_SAND/Data/Secondary_Display_KPI_External_Targets.xlsx
@@ -10,6 +10,12 @@
   <sheets>
     <sheet name="Secondary_Display" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Secondary_Display!$A$1:$M$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Secondary_Display!$A$1:$M$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Secondary_Display!$A$1:$M$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Secondary_Display!$A$1:$M$12</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
   <si>
     <t xml:space="preserve">Store Number</t>
   </si>
@@ -61,73 +67,88 @@
     <t xml:space="preserve">END_DATE</t>
   </si>
   <si>
-    <t xml:space="preserve">IND Grocery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oberon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mawhoods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A3</t>
+    <t xml:space="preserve">0019000001hGaeiAAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gondola End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673822109, 9300673916280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673916969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0019000001hGadgAAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other0007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0019000001hGaeeAAC</t>
   </si>
   <si>
     <t xml:space="preserve">Floor Bin</t>
   </si>
   <si>
-    <t xml:space="preserve">9300673834355</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673836397</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673808172, 9300673800000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pharmacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other0019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673854407, 9300673916792</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673923936, 9300673822109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Castlecrag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Romeos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gondola End</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673840134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9403099004590, Irrelevant0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673923936</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9300673838773</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9403099004590, 9300673840134</t>
+    <t xml:space="preserve">9300673838940, 9300673818027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9310130864900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0019000001hGb52AAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673801036, 9300673843197, 9300673808172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9310042275382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0019000001hGaeSAAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0019000001hGadeAAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673891976, 9300673840479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673828064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0019000001hGaerAAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9310130861817, 9310130115095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9310130317307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0019000001hGaeYAAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673840646, 9300673839794, 9300673840479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9310130860827, 9310130710429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0019000001hGadfAAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9300673839794</t>
   </si>
 </sst>
 </file>
@@ -249,69 +270,53 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -387,28 +392,41 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:5"/>
+  <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="3" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="2" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="4" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="5" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="4" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="5" width="11.0714285714286"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -450,143 +468,290 @@
       </c>
       <c r="AMJ1" s="5"/>
     </row>
-    <row r="2" s="5" customFormat="true" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
+      <c r="K2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="L2" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M2" s="10" t="n">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="J3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="15" t="n">
-        <v>43648</v>
-      </c>
-      <c r="M2" s="15" t="n">
-        <v>43682</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10"/>
-      <c r="B3" s="14" t="s">
+      <c r="K3" s="5"/>
+      <c r="L3" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M3" s="10" t="n">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="10" t="s">
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M4" s="10" t="n">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13" t="s">
+      <c r="I5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M5" s="10" t="n">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="15" t="n">
-        <v>43648</v>
-      </c>
-      <c r="M3" s="15" t="n">
-        <v>43682</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="I6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M6" s="10" t="n">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M7" s="10" t="n">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="I8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M8" s="10" t="n">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M9" s="10" t="n">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M10" s="10" t="n">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M11" s="10" t="n">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="15" t="n">
-        <v>43648</v>
-      </c>
-      <c r="M4" s="15" t="n">
-        <v>43682</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="I12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="15" t="n">
-        <v>43648</v>
-      </c>
-      <c r="M5" s="15" t="n">
-        <v>43682</v>
+      <c r="L12" s="10" t="n">
+        <v>43648</v>
+      </c>
+      <c r="M12" s="10" t="n">
+        <v>43830</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M12"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -594,5 +759,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>